<commit_message>
update UI after discuss
</commit_message>
<xml_diff>
--- a/doc/界面示意图.xlsx
+++ b/doc/界面示意图.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\myWorks\进销存\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\myWorks\进销存\IMS\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Storage" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="99">
   <si>
     <t>SN</t>
   </si>
@@ -193,9 +193,6 @@
   </si>
   <si>
     <t>Sell Return Date</t>
-  </si>
-  <si>
-    <t>？有没有部分退货？</t>
   </si>
   <si>
     <t>Inventory</t>
@@ -288,13 +285,83 @@
   </si>
   <si>
     <t>状态：待确定，待补货，已补货，删除</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>ABC123</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>sn</t>
+  </si>
+  <si>
+    <t>Tribul</t>
+  </si>
+  <si>
+    <r>
+      <t>待定：-- 智能</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>快速输入产品</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>的方法： 
+1、输入产品编码，输入字符后，根据输入字符匹配出可选编码（类似输入法智能联想）
+2、输入产品名称，输入部分字符后，根据输入字符匹配出可选产品，如果只有一个，就自动带出</t>
+    </r>
+  </si>
+  <si>
+    <t>..</t>
+  </si>
+  <si>
+    <t>Quantity In Stock</t>
+  </si>
+  <si>
+    <t>客户</t>
+  </si>
+  <si>
+    <t>考虑：退货可以合并到原货架(仓库)上，也可以放到新货架(仓库)上,数量重新输入</t>
+  </si>
+  <si>
+    <t>Inventory by Product</t>
+  </si>
+  <si>
+    <t>价格计算方式：加权平均值，最新入库价格</t>
+  </si>
+  <si>
+    <t>last_Price_Purchase</t>
+  </si>
+  <si>
+    <t>last_Price_FOB_Ontario</t>
+  </si>
+  <si>
+    <t>Safe_Quantity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -352,8 +419,15 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -369,6 +443,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -482,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -520,9 +600,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -534,9 +611,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -546,15 +620,24 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -848,10 +931,119 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="161905" cy="209524"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1362075" y="6819900"/>
+          <a:ext cx="161905" cy="209524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="161905" cy="209524"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1352550" y="6496050"/>
+          <a:ext cx="161905" cy="209524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>28190</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>133086</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9039225" y="3324225"/>
+          <a:ext cx="3076190" cy="2114286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -949,7 +1141,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1310,10 +1502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R33"/>
+  <dimension ref="B1:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1327,9 +1519,13 @@
     <col min="10" max="10" width="18.140625" customWidth="1"/>
     <col min="11" max="11" width="22.140625" customWidth="1"/>
     <col min="12" max="12" width="16.28515625" customWidth="1"/>
-    <col min="13" max="13" width="38.85546875" customWidth="1"/>
+    <col min="13" max="13" width="23.7109375" customWidth="1"/>
     <col min="14" max="14" width="11.7109375" customWidth="1"/>
-    <col min="17" max="17" width="19.28515625" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" customWidth="1"/>
+    <col min="17" max="17" width="18.42578125" customWidth="1"/>
+    <col min="18" max="18" width="10.5703125" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" customWidth="1"/>
+    <col min="20" max="20" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:18">
@@ -1404,10 +1600,10 @@
       <c r="G4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="34" t="s">
         <v>33</v>
       </c>
       <c r="J4" s="6">
@@ -1425,11 +1621,11 @@
       <c r="N4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="O4" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="P4" s="6">
-        <v>203</v>
+      <c r="P4" s="34">
+        <v>23</v>
       </c>
       <c r="Q4" s="6">
         <v>300</v>
@@ -1465,8 +1661,8 @@
       </c>
     </row>
     <row r="8" spans="2:18" ht="15.75" thickBot="1">
-      <c r="B8" s="25"/>
-      <c r="C8" s="26"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1540,19 +1736,19 @@
       <c r="I13" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J13" s="22" t="s">
+      <c r="J13" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="K13" s="23" t="s">
+      <c r="K13" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="L13" s="23" t="s">
+      <c r="L13" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="M13" s="23" t="s">
+      <c r="M13" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="N13" s="23" t="s">
+      <c r="N13" s="21" t="s">
         <v>11</v>
       </c>
       <c r="O13" s="8" t="s">
@@ -1579,7 +1775,7 @@
       <c r="G14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H14" s="24" t="s">
+      <c r="H14" s="22" t="s">
         <v>44</v>
       </c>
       <c r="I14" s="6" t="s">
@@ -1624,13 +1820,13 @@
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
     </row>
-    <row r="18" spans="2:17">
+    <row r="18" spans="2:19">
       <c r="B18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="2:17" ht="15.75" thickBot="1"/>
-    <row r="20" spans="2:17" ht="26.25" thickBot="1">
+    <row r="19" spans="2:19" ht="15.75" thickBot="1"/>
+    <row r="20" spans="2:19" ht="26.25" thickBot="1">
       <c r="B20" s="2"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8" t="s">
@@ -1645,22 +1841,22 @@
       <c r="G20" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H20" s="23" t="s">
+      <c r="H20" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="I20" s="23" t="s">
+      <c r="I20" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="J20" s="23" t="s">
+      <c r="J20" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="K20" s="23" t="s">
+      <c r="K20" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="L20" s="23" t="s">
+      <c r="L20" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="M20" s="23" t="s">
+      <c r="M20" s="21" t="s">
         <v>10</v>
       </c>
       <c r="N20" s="8" t="s">
@@ -1673,7 +1869,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="2:17" ht="25.5" customHeight="1">
+    <row r="21" spans="2:19" ht="25.5" customHeight="1">
       <c r="B21" s="5" t="s">
         <v>14</v>
       </c>
@@ -1690,7 +1886,7 @@
       <c r="G21" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H21" s="24" t="s">
+      <c r="H21" s="22" t="s">
         <v>44</v>
       </c>
       <c r="I21" s="6" t="s">
@@ -1716,7 +1912,7 @@
       </c>
       <c r="P21" s="6"/>
     </row>
-    <row r="22" spans="2:17" ht="25.5" customHeight="1">
+    <row r="22" spans="2:19" ht="25.5" customHeight="1">
       <c r="B22" s="3" t="s">
         <v>14</v>
       </c>
@@ -1735,18 +1931,13 @@
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
     </row>
-    <row r="24" spans="2:17">
-      <c r="B24" t="s">
+    <row r="26" spans="2:19">
+      <c r="B26" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="2:17">
-      <c r="B26" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="2:17" ht="15.75" thickBot="1"/>
-    <row r="28" spans="2:17" ht="26.25" thickBot="1">
+    <row r="27" spans="2:19" ht="15.75" thickBot="1"/>
+    <row r="28" spans="2:19" ht="39" thickBot="1">
       <c r="B28" s="2"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8" t="s">
@@ -1782,17 +1973,23 @@
       <c r="N28" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="O28" s="9" t="s">
+      <c r="O28" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="P28" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q28" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="P28" s="8" t="s">
+      <c r="R28" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="Q28" s="8" t="s">
+      <c r="S28" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="2:17" ht="25.5" customHeight="1">
+    <row r="29" spans="2:19" ht="25.5" customHeight="1">
       <c r="B29" s="5" t="s">
         <v>14</v>
       </c>
@@ -1806,20 +2003,20 @@
       <c r="F29" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G29" s="24" t="s">
+      <c r="G29" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="H29" s="6" t="s">
+      <c r="H29" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="I29" s="6" t="s">
+      <c r="I29" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="J29" s="6">
+      <c r="J29" s="34">
         <v>203</v>
       </c>
       <c r="K29" s="6">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="L29" s="6"/>
       <c r="M29" s="6">
@@ -1828,17 +2025,23 @@
       <c r="N29" s="6">
         <v>13</v>
       </c>
-      <c r="O29" s="6" t="s">
+      <c r="O29" s="6">
+        <v>10.5</v>
+      </c>
+      <c r="P29" s="6">
+        <v>13</v>
+      </c>
+      <c r="Q29" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="P29" s="6">
+      <c r="R29" s="6">
         <v>0.01</v>
       </c>
-      <c r="Q29" s="6" t="s">
+      <c r="S29" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="2:17" ht="25.5" customHeight="1">
+    <row r="30" spans="2:19" ht="25.5" customHeight="1">
       <c r="B30" s="3" t="s">
         <v>14</v>
       </c>
@@ -1852,24 +2055,110 @@
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="M30" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="M30" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="N30" s="4" t="s">
-        <v>57</v>
-      </c>
+      <c r="N30" s="4"/>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
-    </row>
-    <row r="33" spans="2:5">
-      <c r="B33" t="s">
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+    </row>
+    <row r="32" spans="2:19">
+      <c r="B32" t="s">
+        <v>94</v>
+      </c>
+      <c r="M32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" ht="15.75" thickBot="1"/>
+    <row r="34" spans="2:12" ht="26.25" thickBot="1">
+      <c r="B34" s="2"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J34" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K34" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L34" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" ht="25.5" customHeight="1">
+      <c r="B35" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="5"/>
+      <c r="D35" s="6">
+        <v>1</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G35" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="H35" s="6">
+        <v>50</v>
+      </c>
+      <c r="I35" s="6">
+        <v>100</v>
+      </c>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6">
+        <v>10.5</v>
+      </c>
+      <c r="L35" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" ht="25.5" customHeight="1">
+      <c r="B36" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+    </row>
+    <row r="39" spans="2:12">
+      <c r="B39" t="s">
+        <v>82</v>
+      </c>
+      <c r="E39" t="s">
         <v>83</v>
-      </c>
-      <c r="E33" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1883,8 +2172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q25"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1894,10 +2183,12 @@
     <col min="5" max="5" width="7.140625" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" customWidth="1"/>
     <col min="7" max="7" width="34.5703125" customWidth="1"/>
+    <col min="8" max="8" width="3" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="24.75" customHeight="1">
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1929,59 +2220,61 @@
         <v>43</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="J5" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
-      <c r="Q5" s="27"/>
+      <c r="J5" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="30"/>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="30"/>
     </row>
     <row r="6" spans="2:17" ht="8.25" customHeight="1">
       <c r="C6" s="12"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="27"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
     </row>
     <row r="7" spans="2:17" ht="24" customHeight="1">
       <c r="C7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="27"/>
+      <c r="D7" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="30"/>
     </row>
     <row r="8" spans="2:17" ht="8.25" customHeight="1">
       <c r="C8" s="12"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="27"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="27"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="30"/>
     </row>
     <row r="9" spans="2:17" ht="24" customHeight="1">
       <c r="C9" s="11" t="s">
@@ -1992,15 +2285,17 @@
       <c r="F9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="27"/>
+      <c r="G9" s="14">
+        <v>230</v>
+      </c>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="30"/>
     </row>
     <row r="10" spans="2:17" ht="8.25" customHeight="1">
       <c r="C10" s="12"/>
@@ -2043,10 +2338,13 @@
       <c r="C15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="I15" s="33" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="16" spans="2:17" ht="8.25" customHeight="1">
       <c r="C16" s="12"/>
@@ -2073,10 +2371,10 @@
       <c r="C19" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
     </row>
     <row r="20" spans="3:7" ht="24" customHeight="1">
       <c r="C20" s="12"/>
@@ -2084,14 +2382,14 @@
       <c r="E20" s="13"/>
     </row>
     <row r="21" spans="3:7" ht="24" customHeight="1">
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="18" t="s">
         <v>46</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
     </row>
     <row r="22" spans="3:7" ht="24" customHeight="1">
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="18" t="s">
         <v>47</v>
       </c>
       <c r="D22" s="13"/>
@@ -2103,7 +2401,7 @@
       <c r="E23" s="13"/>
     </row>
     <row r="24" spans="3:7" ht="24" customHeight="1">
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="18" t="s">
         <v>51</v>
       </c>
       <c r="D24" s="13"/>
@@ -2123,15 +2421,16 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G23"/>
+  <dimension ref="B1:G33"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2144,7 +2443,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="24.75" customHeight="1">
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2205,14 +2504,10 @@
     </row>
     <row r="10" spans="2:7" ht="24" customHeight="1">
       <c r="C10" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="20"/>
+        <v>91</v>
+      </c>
+      <c r="D10" s="19"/>
       <c r="E10" s="13"/>
-      <c r="F10" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="20"/>
     </row>
     <row r="11" spans="2:7" ht="8.25" customHeight="1">
       <c r="C11" s="12"/>
@@ -2221,12 +2516,14 @@
     </row>
     <row r="12" spans="2:7" ht="24" customHeight="1">
       <c r="C12" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
+        <v>7</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="19"/>
     </row>
     <row r="13" spans="2:7" ht="8.25" customHeight="1">
       <c r="C13" s="12"/>
@@ -2235,14 +2532,12 @@
     </row>
     <row r="14" spans="2:7" ht="24" customHeight="1">
       <c r="C14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="20"/>
+        <v>9</v>
+      </c>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
     </row>
     <row r="15" spans="2:7" ht="8.25" customHeight="1">
       <c r="C15" s="12"/>
@@ -2251,61 +2546,106 @@
     </row>
     <row r="16" spans="2:7" ht="24" customHeight="1">
       <c r="C16" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-    </row>
-    <row r="17" spans="2:5" ht="24" customHeight="1">
+        <v>10</v>
+      </c>
+      <c r="D16" s="19"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="19"/>
+    </row>
+    <row r="17" spans="2:7" ht="8.25" customHeight="1">
       <c r="C17" s="12"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
     </row>
-    <row r="18" spans="2:5" ht="24" customHeight="1">
-      <c r="C18" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-    </row>
-    <row r="19" spans="2:5" ht="24" customHeight="1">
-      <c r="C19" s="19" t="s">
-        <v>42</v>
-      </c>
+    <row r="18" spans="2:7" ht="24" customHeight="1">
+      <c r="C18" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+    </row>
+    <row r="19" spans="2:7" ht="24" customHeight="1">
+      <c r="C19" s="12"/>
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
     </row>
-    <row r="20" spans="2:5" ht="24" customHeight="1">
-      <c r="C20" s="19" t="s">
-        <v>49</v>
+    <row r="20" spans="2:7" ht="24" customHeight="1">
+      <c r="C20" s="18" t="s">
+        <v>41</v>
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
     </row>
-    <row r="21" spans="2:5" ht="24" customHeight="1">
-      <c r="B21" s="19"/>
-      <c r="C21" s="19" t="s">
-        <v>48</v>
+    <row r="21" spans="2:7" ht="24" customHeight="1">
+      <c r="C21" s="18" t="s">
+        <v>42</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
     </row>
-    <row r="22" spans="2:5" ht="24" customHeight="1">
-      <c r="C22" s="12"/>
+    <row r="22" spans="2:7" ht="24" customHeight="1">
+      <c r="C22" s="18" t="s">
+        <v>49</v>
+      </c>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
     </row>
-    <row r="23" spans="2:5" ht="18.75">
-      <c r="C23" s="19" t="s">
+    <row r="23" spans="2:7" ht="24" customHeight="1">
+      <c r="B23" s="18"/>
+      <c r="C23" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+    </row>
+    <row r="24" spans="2:7" ht="24" customHeight="1">
+      <c r="C24" s="12"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+    </row>
+    <row r="25" spans="2:7" ht="18.75">
+      <c r="C25" s="18" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="C29" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7">
+      <c r="C31" s="11">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7">
+      <c r="C32" s="11">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4">
+      <c r="C33" s="11">
+        <v>3</v>
+      </c>
+      <c r="D33">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="D18:G18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2316,7 +2656,7 @@
   <dimension ref="B1:G23"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2329,11 +2669,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="24.75" customHeight="1">
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>52</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="24" customHeight="1">
@@ -2395,12 +2735,12 @@
       <c r="C10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="20"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="13"/>
       <c r="F10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="20"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" spans="2:7" ht="8.25" customHeight="1">
       <c r="C11" s="12"/>
@@ -2411,10 +2751,10 @@
       <c r="C12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
     </row>
     <row r="13" spans="2:7" ht="8.25" customHeight="1">
       <c r="C13" s="12"/>
@@ -2425,12 +2765,12 @@
       <c r="C14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="20"/>
+      <c r="D14" s="14"/>
       <c r="E14" s="13"/>
       <c r="F14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="20"/>
+      <c r="G14" s="14"/>
     </row>
     <row r="15" spans="2:7" ht="8.25" customHeight="1">
       <c r="C15" s="12"/>
@@ -2441,10 +2781,10 @@
       <c r="C16" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
     </row>
     <row r="17" spans="2:5" ht="24" customHeight="1">
       <c r="C17" s="12"/>
@@ -2452,30 +2792,30 @@
       <c r="E17" s="13"/>
     </row>
     <row r="18" spans="2:5" ht="24" customHeight="1">
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="18" t="s">
         <v>41</v>
       </c>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
     </row>
     <row r="19" spans="2:5" ht="24" customHeight="1">
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="18" t="s">
         <v>42</v>
       </c>
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
     </row>
     <row r="20" spans="2:5" ht="24" customHeight="1">
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="18" t="s">
         <v>49</v>
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
     </row>
     <row r="21" spans="2:5" ht="24" customHeight="1">
-      <c r="B21" s="19"/>
-      <c r="C21" s="19" t="s">
-        <v>48</v>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18" t="s">
+        <v>93</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
@@ -2486,7 +2826,7 @@
       <c r="E22" s="13"/>
     </row>
     <row r="23" spans="2:5" ht="18.75">
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="18" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2504,53 +2844,56 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="B1:J8"/>
+  <dimension ref="B1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="5" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" customWidth="1"/>
+    <col min="4" max="6" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="24.85546875" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10">
+    <row r="1" spans="2:11">
       <c r="B1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="2:10" ht="15.75" thickBot="1"/>
-    <row r="3" spans="2:10" ht="26.25" thickBot="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" ht="15.75" thickBot="1"/>
+    <row r="3" spans="2:11" ht="26.25" thickBot="1">
       <c r="B3" s="2"/>
       <c r="C3" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="K3" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="25.5" customHeight="1">
+    <row r="4" spans="2:11" ht="25.5" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
@@ -2561,25 +2904,28 @@
         <v>43206</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="32">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="6">
+      <c r="I4" s="6">
         <v>13</v>
       </c>
-      <c r="I4" s="6">
+      <c r="J4" s="6">
         <v>100</v>
       </c>
-      <c r="J4" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" ht="25.5" customHeight="1">
+      <c r="K4" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="25.5" customHeight="1">
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
@@ -2590,29 +2936,33 @@
         <v>43206</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="32">
+        <v>2</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="H5" s="6">
+      <c r="I5" s="6">
         <v>45</v>
       </c>
-      <c r="I5" s="6">
+      <c r="J5" s="6">
         <v>30</v>
       </c>
-      <c r="J5" s="6"/>
-    </row>
-    <row r="8" spans="2:10">
+      <c r="K5" s="6"/>
+    </row>
+    <row r="8" spans="2:11">
       <c r="B8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2624,7 +2974,7 @@
   <dimension ref="B1:Q33"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2637,22 +2987,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="24.75" customHeight="1">
-      <c r="B1" s="18" t="s">
-        <v>59</v>
+      <c r="B1" s="17" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="24" customHeight="1">
       <c r="C3" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>38</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" s="28">
+        <v>59</v>
+      </c>
+      <c r="G3" s="25">
         <v>43206</v>
       </c>
     </row>
@@ -2663,12 +3013,12 @@
     </row>
     <row r="5" spans="2:9" ht="24" customHeight="1">
       <c r="C5" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
+        <v>62</v>
+      </c>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
     </row>
     <row r="6" spans="2:9" ht="8.25" customHeight="1">
       <c r="C6" s="12"/>
@@ -2677,14 +3027,14 @@
     </row>
     <row r="7" spans="2:9" ht="24" customHeight="1">
       <c r="C7" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D7" s="14">
         <v>3</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G7" s="14"/>
     </row>
@@ -2697,19 +3047,19 @@
       <c r="C9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
       <c r="I9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="9.75" customHeight="1">
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
     </row>
     <row r="11" spans="2:9" ht="8.25" customHeight="1">
       <c r="C11" s="12"/>
@@ -2720,12 +3070,14 @@
       <c r="C12" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="14"/>
+      <c r="D12" s="14" t="s">
+        <v>85</v>
+      </c>
       <c r="E12" s="13"/>
       <c r="F12" s="11"/>
-      <c r="G12" s="16"/>
-      <c r="I12" s="30" t="s">
-        <v>72</v>
+      <c r="G12" s="15"/>
+      <c r="I12" s="27" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="2:9" ht="8.25" customHeight="1">
@@ -2737,12 +3089,12 @@
       <c r="C14" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
       <c r="I14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="8.25" customHeight="1">
@@ -2752,7 +3104,7 @@
     </row>
     <row r="16" spans="2:9" ht="24" customHeight="1">
       <c r="C16" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="13"/>
@@ -2761,86 +3113,93 @@
       </c>
       <c r="G16" s="14"/>
       <c r="I16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="3:17" ht="8.25" customHeight="1">
       <c r="C17" s="12"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
-      <c r="J17" s="29"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="3:17" ht="24" customHeight="1">
       <c r="C18" s="12"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
     </row>
-    <row r="19" spans="3:17" ht="24" customHeight="1"/>
+    <row r="19" spans="3:17" ht="24" customHeight="1">
+      <c r="I19" t="s">
+        <v>84</v>
+      </c>
+    </row>
     <row r="20" spans="3:17" ht="24" customHeight="1">
-      <c r="J20" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="27"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="27"/>
-      <c r="Q20" s="27"/>
+      <c r="I20" t="s">
+        <v>86</v>
+      </c>
+      <c r="J20" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="30"/>
     </row>
     <row r="21" spans="3:17" ht="24" customHeight="1">
-      <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="27"/>
-      <c r="N21" s="27"/>
-      <c r="O21" s="27"/>
-      <c r="P21" s="27"/>
-      <c r="Q21" s="27"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="30"/>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="30"/>
     </row>
     <row r="22" spans="3:17" ht="24" customHeight="1">
-      <c r="J22" s="27"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="27"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="27"/>
-      <c r="P22" s="27"/>
-      <c r="Q22" s="27"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="30"/>
+      <c r="P22" s="30"/>
+      <c r="Q22" s="30"/>
     </row>
     <row r="23" spans="3:17" ht="24" customHeight="1">
       <c r="C23" s="12"/>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="27"/>
-      <c r="M23" s="27"/>
-      <c r="N23" s="27"/>
-      <c r="O23" s="27"/>
-      <c r="P23" s="27"/>
-      <c r="Q23" s="27"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="30"/>
+      <c r="P23" s="30"/>
+      <c r="Q23" s="30"/>
     </row>
     <row r="24" spans="3:17">
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="27"/>
-      <c r="Q24" s="27"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="30"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="30"/>
     </row>
     <row r="30" spans="3:17" ht="18.75">
-      <c r="C30" s="19" t="s">
+      <c r="C30" s="18" t="s">
         <v>46</v>
       </c>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
     </row>
     <row r="31" spans="3:17" ht="18.75">
-      <c r="C31" s="19" t="s">
-        <v>75</v>
+      <c r="C31" s="18" t="s">
+        <v>74</v>
       </c>
       <c r="D31" s="13"/>
       <c r="E31" s="13"/>
@@ -2851,7 +3210,7 @@
       <c r="E32" s="13"/>
     </row>
     <row r="33" spans="3:5" ht="18.75">
-      <c r="C33" s="19"/>
+      <c r="C33" s="18"/>
       <c r="D33" s="13"/>
       <c r="E33" s="13"/>
     </row>
@@ -2876,7 +3235,7 @@
   <dimension ref="B1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2888,17 +3247,17 @@
   <sheetData>
     <row r="1" spans="2:10">
       <c r="B1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="2:10" ht="15.75" thickBot="1"/>
     <row r="3" spans="2:10" ht="26.25" thickBot="1">
       <c r="B3" s="2"/>
       <c r="C3" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>78</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>79</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>9</v>
@@ -2910,7 +3269,7 @@
         <v>3</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>12</v>
@@ -2930,7 +3289,7 @@
         <v>43206</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>31</v>
@@ -2957,13 +3316,13 @@
         <v>43206</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>68</v>
       </c>
       <c r="H5" s="6">
         <v>45</v>
@@ -2974,8 +3333,8 @@
       <c r="J5" s="6"/>
     </row>
     <row r="8" spans="2:10" ht="20.25">
-      <c r="B8" s="31" t="s">
-        <v>77</v>
+      <c r="B8" s="28" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -3004,22 +3363,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="24.75" customHeight="1">
-      <c r="B1" s="18" t="s">
-        <v>76</v>
+      <c r="B1" s="17" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="24" customHeight="1">
       <c r="C3" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>38</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G3" s="28">
+        <v>78</v>
+      </c>
+      <c r="G3" s="25">
         <v>43206</v>
       </c>
     </row>
@@ -3032,10 +3391,10 @@
       <c r="C5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
     </row>
     <row r="6" spans="2:9" ht="8.25" customHeight="1">
       <c r="C6" s="12"/>
@@ -3044,14 +3403,14 @@
     </row>
     <row r="7" spans="2:9" ht="24" customHeight="1">
       <c r="C7" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D7" s="14">
         <v>3</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G7" s="14"/>
     </row>
@@ -3064,16 +3423,16 @@
       <c r="C9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
     </row>
     <row r="10" spans="2:9" ht="9.75" customHeight="1">
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
     </row>
     <row r="11" spans="2:9" ht="8.25" customHeight="1">
       <c r="C11" s="12"/>
@@ -3087,8 +3446,8 @@
       <c r="D12" s="14"/>
       <c r="E12" s="13"/>
       <c r="F12" s="11"/>
-      <c r="G12" s="16"/>
-      <c r="I12" s="30"/>
+      <c r="G12" s="15"/>
+      <c r="I12" s="27"/>
     </row>
     <row r="13" spans="2:9" ht="8.25" customHeight="1">
       <c r="C13" s="12"/>
@@ -3099,10 +3458,10 @@
       <c r="C14" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
     </row>
     <row r="15" spans="2:9" ht="8.25" customHeight="1">
       <c r="C15" s="12"/>
@@ -3111,7 +3470,7 @@
     </row>
     <row r="16" spans="2:9" ht="24" customHeight="1">
       <c r="C16" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="13"/>
@@ -3124,7 +3483,7 @@
       <c r="C17" s="12"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
-      <c r="J17" s="29"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="3:17" ht="24" customHeight="1">
       <c r="C18" s="12"/>
@@ -3133,69 +3492,69 @@
     </row>
     <row r="19" spans="3:17" ht="24" customHeight="1"/>
     <row r="20" spans="3:17" ht="24" customHeight="1">
-      <c r="J20" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="27"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="27"/>
-      <c r="Q20" s="27"/>
+      <c r="J20" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="K20" s="30"/>
+      <c r="L20" s="30"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="30"/>
     </row>
     <row r="21" spans="3:17" ht="24" customHeight="1">
-      <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="27"/>
-      <c r="N21" s="27"/>
-      <c r="O21" s="27"/>
-      <c r="P21" s="27"/>
-      <c r="Q21" s="27"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="30"/>
+      <c r="L21" s="30"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="30"/>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="30"/>
     </row>
     <row r="22" spans="3:17" ht="24" customHeight="1">
-      <c r="J22" s="27"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="27"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="27"/>
-      <c r="P22" s="27"/>
-      <c r="Q22" s="27"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="30"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
+      <c r="O22" s="30"/>
+      <c r="P22" s="30"/>
+      <c r="Q22" s="30"/>
     </row>
     <row r="23" spans="3:17" ht="24" customHeight="1">
       <c r="C23" s="12"/>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="27"/>
-      <c r="M23" s="27"/>
-      <c r="N23" s="27"/>
-      <c r="O23" s="27"/>
-      <c r="P23" s="27"/>
-      <c r="Q23" s="27"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="30"/>
+      <c r="O23" s="30"/>
+      <c r="P23" s="30"/>
+      <c r="Q23" s="30"/>
     </row>
     <row r="24" spans="3:17">
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="27"/>
-      <c r="Q24" s="27"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="30"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="30"/>
     </row>
     <row r="30" spans="3:17" ht="18.75">
-      <c r="C30" s="19" t="s">
+      <c r="C30" s="18" t="s">
         <v>46</v>
       </c>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
     </row>
     <row r="31" spans="3:17" ht="18.75">
-      <c r="C31" s="19" t="s">
+      <c r="C31" s="18" t="s">
         <v>47</v>
       </c>
       <c r="D31" s="13"/>
@@ -3207,7 +3566,7 @@
       <c r="E32" s="13"/>
     </row>
     <row r="33" spans="3:5" ht="18.75">
-      <c r="C33" s="19"/>
+      <c r="C33" s="18"/>
       <c r="D33" s="13"/>
       <c r="E33" s="13"/>
     </row>

</xml_diff>

<commit_message>
update sql + UI
</commit_message>
<xml_diff>
--- a/doc/界面示意图.xlsx
+++ b/doc/界面示意图.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Storage" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="103">
   <si>
     <t>SN</t>
   </si>
@@ -356,12 +356,24 @@
   <si>
     <t>Safe_Quantity</t>
   </si>
+  <si>
+    <t>Demand Date</t>
+  </si>
+  <si>
+    <t>Urgency degree</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>需备货，已备</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,6 +437,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
     </font>
   </fonts>
   <fills count="5">
@@ -562,7 +579,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -626,6 +643,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -635,9 +655,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1603,7 +1621,7 @@
       <c r="H4" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="34" t="s">
+      <c r="I4" s="31" t="s">
         <v>33</v>
       </c>
       <c r="J4" s="6">
@@ -1621,10 +1639,10 @@
       <c r="N4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="O4" s="34" t="s">
+      <c r="O4" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="P4" s="34">
+      <c r="P4" s="31">
         <v>23</v>
       </c>
       <c r="Q4" s="6">
@@ -2006,13 +2024,13 @@
       <c r="G29" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="H29" s="34" t="s">
+      <c r="H29" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="I29" s="34" t="s">
+      <c r="I29" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="J29" s="34">
+      <c r="J29" s="31">
         <v>203</v>
       </c>
       <c r="K29" s="6">
@@ -2172,8 +2190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2220,61 +2238,61 @@
         <v>43</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="J5" s="30" t="s">
+      <c r="J5" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
-      <c r="O5" s="30"/>
-      <c r="P5" s="30"/>
-      <c r="Q5" s="30"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="33"/>
     </row>
     <row r="6" spans="2:17" ht="8.25" customHeight="1">
       <c r="C6" s="12"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="33"/>
     </row>
     <row r="7" spans="2:17" ht="24" customHeight="1">
       <c r="C7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="33"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="33"/>
     </row>
     <row r="8" spans="2:17" ht="8.25" customHeight="1">
       <c r="C8" s="12"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="30"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="30"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="33"/>
     </row>
     <row r="9" spans="2:17" ht="24" customHeight="1">
       <c r="C9" s="11" t="s">
@@ -2288,14 +2306,14 @@
       <c r="G9" s="14">
         <v>230</v>
       </c>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="33"/>
+      <c r="Q9" s="33"/>
     </row>
     <row r="10" spans="2:17" ht="8.25" customHeight="1">
       <c r="C10" s="12"/>
@@ -2338,11 +2356,11 @@
       <c r="C15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="I15" s="33" t="s">
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="I15" s="30" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2371,10 +2389,10 @@
       <c r="C19" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
     </row>
     <row r="20" spans="3:7" ht="24" customHeight="1">
       <c r="C20" s="12"/>
@@ -2534,10 +2552,10 @@
       <c r="C14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
     </row>
     <row r="15" spans="2:7" ht="8.25" customHeight="1">
       <c r="C15" s="12"/>
@@ -2564,10 +2582,10 @@
       <c r="C18" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
     </row>
     <row r="19" spans="2:7" ht="24" customHeight="1">
       <c r="C19" s="12"/>
@@ -2751,10 +2769,10 @@
       <c r="C12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
     </row>
     <row r="13" spans="2:7" ht="8.25" customHeight="1">
       <c r="C13" s="12"/>
@@ -2781,10 +2799,10 @@
       <c r="C16" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
     </row>
     <row r="17" spans="2:5" ht="24" customHeight="1">
       <c r="C17" s="12"/>
@@ -2906,7 +2924,7 @@
       <c r="E4" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="32">
+      <c r="F4" s="29">
         <v>1</v>
       </c>
       <c r="G4" s="6" t="s">
@@ -2938,7 +2956,7 @@
       <c r="E5" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F5" s="32">
+      <c r="F5" s="29">
         <v>2</v>
       </c>
       <c r="G5" s="6" t="s">
@@ -3015,10 +3033,10 @@
       <c r="C5" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
     </row>
     <row r="6" spans="2:9" ht="8.25" customHeight="1">
       <c r="C6" s="12"/>
@@ -3047,10 +3065,10 @@
       <c r="C9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
       <c r="I9" t="s">
         <v>70</v>
       </c>
@@ -3089,10 +3107,10 @@
       <c r="C14" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
       <c r="I14" t="s">
         <v>73</v>
       </c>
@@ -3136,59 +3154,59 @@
       <c r="I20" t="s">
         <v>86</v>
       </c>
-      <c r="J20" s="30" t="s">
+      <c r="J20" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="K20" s="30"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="30"/>
-      <c r="P20" s="30"/>
-      <c r="Q20" s="30"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="33"/>
+      <c r="O20" s="33"/>
+      <c r="P20" s="33"/>
+      <c r="Q20" s="33"/>
     </row>
     <row r="21" spans="3:17" ht="24" customHeight="1">
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="30"/>
-      <c r="P21" s="30"/>
-      <c r="Q21" s="30"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="33"/>
+      <c r="O21" s="33"/>
+      <c r="P21" s="33"/>
+      <c r="Q21" s="33"/>
     </row>
     <row r="22" spans="3:17" ht="24" customHeight="1">
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="30"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="30"/>
-      <c r="O22" s="30"/>
-      <c r="P22" s="30"/>
-      <c r="Q22" s="30"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="33"/>
+      <c r="O22" s="33"/>
+      <c r="P22" s="33"/>
+      <c r="Q22" s="33"/>
     </row>
     <row r="23" spans="3:17" ht="24" customHeight="1">
       <c r="C23" s="12"/>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
-      <c r="J23" s="30"/>
-      <c r="K23" s="30"/>
-      <c r="L23" s="30"/>
-      <c r="M23" s="30"/>
-      <c r="N23" s="30"/>
-      <c r="O23" s="30"/>
-      <c r="P23" s="30"/>
-      <c r="Q23" s="30"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="33"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="33"/>
+      <c r="O23" s="33"/>
+      <c r="P23" s="33"/>
+      <c r="Q23" s="33"/>
     </row>
     <row r="24" spans="3:17">
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="30"/>
-      <c r="O24" s="30"/>
-      <c r="P24" s="30"/>
-      <c r="Q24" s="30"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="33"/>
+      <c r="O24" s="33"/>
+      <c r="P24" s="33"/>
+      <c r="Q24" s="33"/>
     </row>
     <row r="30" spans="3:17" ht="18.75">
       <c r="C30" s="18" t="s">
@@ -3232,10 +3250,10 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="B1:J8"/>
+  <dimension ref="B1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3245,13 +3263,13 @@
     <col min="10" max="10" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10">
+    <row r="1" spans="2:11">
       <c r="B1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="15.75" thickBot="1"/>
-    <row r="3" spans="2:10" ht="26.25" thickBot="1">
+    <row r="2" spans="2:11" ht="15.75" thickBot="1"/>
+    <row r="3" spans="2:11" ht="26.25" thickBot="1">
       <c r="B3" s="2"/>
       <c r="C3" s="8" t="s">
         <v>77</v>
@@ -3278,7 +3296,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="25.5" customHeight="1">
+    <row r="4" spans="2:11" ht="25.5" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
@@ -3305,7 +3323,7 @@
       </c>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="2:10" ht="25.5" customHeight="1">
+    <row r="5" spans="2:11" ht="25.5" customHeight="1">
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
@@ -3332,13 +3350,50 @@
       </c>
       <c r="J5" s="6"/>
     </row>
-    <row r="8" spans="2:10" ht="20.25">
+    <row r="8" spans="2:11" ht="20.25">
       <c r="B8" s="28" t="s">
         <v>76</v>
       </c>
     </row>
+    <row r="9" spans="2:11" ht="15.75" thickBot="1"/>
+    <row r="10" spans="2:11" ht="26.25" thickBot="1">
+      <c r="B10" s="2"/>
+      <c r="C10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11">
+      <c r="J11" s="35" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3391,10 +3446,10 @@
       <c r="C5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
     </row>
     <row r="6" spans="2:9" ht="8.25" customHeight="1">
       <c r="C6" s="12"/>
@@ -3423,10 +3478,10 @@
       <c r="C9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
     </row>
     <row r="10" spans="2:9" ht="9.75" customHeight="1">
       <c r="D10" s="16"/>
@@ -3458,10 +3513,10 @@
       <c r="C14" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
     </row>
     <row r="15" spans="2:9" ht="8.25" customHeight="1">
       <c r="C15" s="12"/>
@@ -3492,59 +3547,59 @@
     </row>
     <row r="19" spans="3:17" ht="24" customHeight="1"/>
     <row r="20" spans="3:17" ht="24" customHeight="1">
-      <c r="J20" s="30" t="s">
+      <c r="J20" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="K20" s="30"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="30"/>
-      <c r="P20" s="30"/>
-      <c r="Q20" s="30"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="33"/>
+      <c r="O20" s="33"/>
+      <c r="P20" s="33"/>
+      <c r="Q20" s="33"/>
     </row>
     <row r="21" spans="3:17" ht="24" customHeight="1">
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="30"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="30"/>
-      <c r="P21" s="30"/>
-      <c r="Q21" s="30"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="33"/>
+      <c r="O21" s="33"/>
+      <c r="P21" s="33"/>
+      <c r="Q21" s="33"/>
     </row>
     <row r="22" spans="3:17" ht="24" customHeight="1">
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="30"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="30"/>
-      <c r="O22" s="30"/>
-      <c r="P22" s="30"/>
-      <c r="Q22" s="30"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="33"/>
+      <c r="O22" s="33"/>
+      <c r="P22" s="33"/>
+      <c r="Q22" s="33"/>
     </row>
     <row r="23" spans="3:17" ht="24" customHeight="1">
       <c r="C23" s="12"/>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
-      <c r="J23" s="30"/>
-      <c r="K23" s="30"/>
-      <c r="L23" s="30"/>
-      <c r="M23" s="30"/>
-      <c r="N23" s="30"/>
-      <c r="O23" s="30"/>
-      <c r="P23" s="30"/>
-      <c r="Q23" s="30"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="33"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="33"/>
+      <c r="O23" s="33"/>
+      <c r="P23" s="33"/>
+      <c r="Q23" s="33"/>
     </row>
     <row r="24" spans="3:17">
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="30"/>
-      <c r="O24" s="30"/>
-      <c r="P24" s="30"/>
-      <c r="Q24" s="30"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="33"/>
+      <c r="O24" s="33"/>
+      <c r="P24" s="33"/>
+      <c r="Q24" s="33"/>
     </row>
     <row r="30" spans="3:17" ht="18.75">
       <c r="C30" s="18" t="s">

</xml_diff>

<commit_message>
add Sampling and customer fold
</commit_message>
<xml_diff>
--- a/doc/界面示意图.xlsx
+++ b/doc/界面示意图.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Storage" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="104">
   <si>
     <t>SN</t>
   </si>
@@ -248,15 +248,9 @@
     <t>选定产品后，自动从数据库中抓取数据提示给销售员。</t>
   </si>
   <si>
-    <t>1，供货商报价区间</t>
-  </si>
-  <si>
     <t>3，库存批次信息列表(批号，数量，库房，供应商)</t>
   </si>
   <si>
-    <t>2，近三个月本人的报给客户价格区间</t>
-  </si>
-  <si>
     <t>选择客户</t>
   </si>
   <si>
@@ -288,9 +282,6 @@
   </si>
   <si>
     <t>+</t>
-  </si>
-  <si>
-    <t>ABC123</t>
   </si>
   <si>
     <t>-</t>
@@ -368,12 +359,24 @@
   <si>
     <t>需备货，已备</t>
   </si>
+  <si>
+    <t>WWBE</t>
+  </si>
+  <si>
+    <t>White Willow</t>
+  </si>
+  <si>
+    <t>1，供货商报价区间    $10  - $12</t>
+  </si>
+  <si>
+    <t>2，近三个月本人的报给客户价格区间  $12 - $15.50</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -442,6 +445,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -579,7 +590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -646,6 +657,7 @@
     <xf numFmtId="1" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -655,7 +667,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1156,6 +1168,82 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>94384</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>76004</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9077325" y="6257925"/>
+          <a:ext cx="6923809" cy="1571429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>295275</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>313906</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>304696</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2638425" y="2562225"/>
+          <a:ext cx="3352381" cy="828571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1992,10 +2080,10 @@
         <v>6</v>
       </c>
       <c r="O28" s="8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="P28" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="Q28" s="9" t="s">
         <v>7</v>
@@ -2087,10 +2175,10 @@
     </row>
     <row r="32" spans="2:19">
       <c r="B32" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="M32" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="2:12" ht="15.75" thickBot="1"/>
@@ -2110,7 +2198,7 @@
         <v>43</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I34" s="8" t="s">
         <v>12</v>
@@ -2173,10 +2261,10 @@
     </row>
     <row r="39" spans="2:12">
       <c r="B39" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E39" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2238,61 +2326,61 @@
         <v>43</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="J5" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="33"/>
+      <c r="J5" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34"/>
     </row>
     <row r="6" spans="2:17" ht="8.25" customHeight="1">
       <c r="C6" s="12"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="33"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="34"/>
     </row>
     <row r="7" spans="2:17" ht="24" customHeight="1">
       <c r="C7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
+      <c r="D7" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="34"/>
     </row>
     <row r="8" spans="2:17" ht="8.25" customHeight="1">
       <c r="C8" s="12"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="33"/>
-      <c r="Q8" s="33"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="34"/>
+      <c r="Q8" s="34"/>
     </row>
     <row r="9" spans="2:17" ht="24" customHeight="1">
       <c r="C9" s="11" t="s">
@@ -2306,14 +2394,14 @@
       <c r="G9" s="14">
         <v>230</v>
       </c>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="33"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="33"/>
-      <c r="Q9" s="33"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="34"/>
     </row>
     <row r="10" spans="2:17" ht="8.25" customHeight="1">
       <c r="C10" s="12"/>
@@ -2356,12 +2444,12 @@
       <c r="C15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
       <c r="I15" s="30" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="2:17" ht="8.25" customHeight="1">
@@ -2389,10 +2477,10 @@
       <c r="C19" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
     </row>
     <row r="20" spans="3:7" ht="24" customHeight="1">
       <c r="C20" s="12"/>
@@ -2522,7 +2610,7 @@
     </row>
     <row r="10" spans="2:7" ht="24" customHeight="1">
       <c r="C10" s="11" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="13"/>
@@ -2552,10 +2640,10 @@
       <c r="C14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
     </row>
     <row r="15" spans="2:7" ht="8.25" customHeight="1">
       <c r="C15" s="12"/>
@@ -2582,10 +2670,10 @@
       <c r="C18" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
     </row>
     <row r="19" spans="2:7" ht="24" customHeight="1">
       <c r="C19" s="12"/>
@@ -2633,7 +2721,7 @@
     </row>
     <row r="29" spans="2:7">
       <c r="C29" s="11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="2:7">
@@ -2769,10 +2857,10 @@
       <c r="C12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
     </row>
     <row r="13" spans="2:7" ht="8.25" customHeight="1">
       <c r="C13" s="12"/>
@@ -2799,10 +2887,10 @@
       <c r="C16" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
     </row>
     <row r="17" spans="2:5" ht="24" customHeight="1">
       <c r="C17" s="12"/>
@@ -2833,7 +2921,7 @@
     <row r="21" spans="2:5" ht="24" customHeight="1">
       <c r="B21" s="18"/>
       <c r="C21" s="18" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
@@ -2893,7 +2981,7 @@
         <v>62</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>2</v>
@@ -2975,7 +3063,7 @@
     </row>
     <row r="8" spans="2:11">
       <c r="B8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2989,10 +3077,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="B1:Q33"/>
+  <dimension ref="B1:R33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3004,12 +3092,12 @@
     <col min="7" max="7" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="24.75" customHeight="1">
+    <row r="1" spans="2:10" ht="24.75" customHeight="1">
       <c r="B1" s="17" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="24" customHeight="1">
+    <row r="3" spans="2:10" ht="24" customHeight="1">
       <c r="C3" s="11" t="s">
         <v>65</v>
       </c>
@@ -3024,26 +3112,26 @@
         <v>43206</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="8.25" customHeight="1">
+    <row r="4" spans="2:10" ht="8.25" customHeight="1">
       <c r="C4" s="12"/>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
     </row>
-    <row r="5" spans="2:9" ht="24" customHeight="1">
+    <row r="5" spans="2:10" ht="24" customHeight="1">
       <c r="C5" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-    </row>
-    <row r="6" spans="2:9" ht="8.25" customHeight="1">
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+    </row>
+    <row r="6" spans="2:10" ht="8.25" customHeight="1">
       <c r="C6" s="12"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
     </row>
-    <row r="7" spans="2:9" ht="24" customHeight="1">
+    <row r="7" spans="2:10" ht="24" customHeight="1">
       <c r="C7" s="11" t="s">
         <v>68</v>
       </c>
@@ -3056,173 +3144,178 @@
       </c>
       <c r="G7" s="14"/>
     </row>
-    <row r="8" spans="2:9" ht="8.25" customHeight="1">
+    <row r="8" spans="2:10" ht="8.25" customHeight="1">
       <c r="C8" s="12"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
     </row>
-    <row r="9" spans="2:9" ht="24" customHeight="1">
+    <row r="9" spans="2:10" ht="24" customHeight="1">
       <c r="C9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="I9" t="s">
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="J9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="9.75" customHeight="1">
+    <row r="10" spans="2:10" ht="9.75" customHeight="1">
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
     </row>
-    <row r="11" spans="2:9" ht="8.25" customHeight="1">
+    <row r="11" spans="2:10" ht="8.25" customHeight="1">
       <c r="C11" s="12"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
     </row>
-    <row r="12" spans="2:9" ht="24" customHeight="1">
+    <row r="12" spans="2:10" ht="24" customHeight="1">
       <c r="C12" s="11" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="11"/>
       <c r="G12" s="15"/>
-      <c r="I12" s="27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" ht="8.25" customHeight="1">
+      <c r="I12" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="J12" s="27" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="8.25" customHeight="1">
       <c r="C13" s="12"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
     </row>
-    <row r="14" spans="2:9" ht="24" customHeight="1">
+    <row r="14" spans="2:10" ht="24" customHeight="1">
       <c r="C14" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="I14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" ht="8.25" customHeight="1">
+      <c r="D14" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="I14" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="J14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="8.25" customHeight="1">
       <c r="C15" s="12"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
     </row>
-    <row r="16" spans="2:9" ht="24" customHeight="1">
+    <row r="16" spans="2:10" ht="24" customHeight="1">
       <c r="C16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="14"/>
+      <c r="D16" s="14">
+        <v>15</v>
+      </c>
       <c r="E16" s="13"/>
       <c r="F16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="14"/>
-      <c r="I16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="3:17" ht="8.25" customHeight="1">
+      <c r="G16" s="14">
+        <v>50</v>
+      </c>
+      <c r="J16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="3:18" ht="8.25" customHeight="1">
       <c r="C17" s="12"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
-      <c r="J17" s="26"/>
-    </row>
-    <row r="18" spans="3:17" ht="24" customHeight="1">
+      <c r="K17" s="26"/>
+    </row>
+    <row r="18" spans="3:18" ht="24" customHeight="1">
       <c r="C18" s="12"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
     </row>
-    <row r="19" spans="3:17" ht="24" customHeight="1">
-      <c r="I19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="3:17" ht="24" customHeight="1">
-      <c r="I20" t="s">
-        <v>86</v>
-      </c>
-      <c r="J20" s="33" t="s">
+    <row r="19" spans="3:18" ht="24" customHeight="1"/>
+    <row r="20" spans="3:18" ht="24" customHeight="1">
+      <c r="K20" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="33"/>
-      <c r="P20" s="33"/>
-      <c r="Q20" s="33"/>
-    </row>
-    <row r="21" spans="3:17" ht="24" customHeight="1">
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33"/>
-      <c r="O21" s="33"/>
-      <c r="P21" s="33"/>
-      <c r="Q21" s="33"/>
-    </row>
-    <row r="22" spans="3:17" ht="24" customHeight="1">
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="33"/>
-      <c r="Q22" s="33"/>
-    </row>
-    <row r="23" spans="3:17" ht="24" customHeight="1">
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="34"/>
+      <c r="P20" s="34"/>
+      <c r="Q20" s="34"/>
+      <c r="R20" s="34"/>
+    </row>
+    <row r="21" spans="3:18" ht="24" customHeight="1">
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="34"/>
+      <c r="P21" s="34"/>
+      <c r="Q21" s="34"/>
+      <c r="R21" s="34"/>
+    </row>
+    <row r="22" spans="3:18" ht="24" customHeight="1">
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="34"/>
+      <c r="P22" s="34"/>
+      <c r="Q22" s="34"/>
+      <c r="R22" s="34"/>
+    </row>
+    <row r="23" spans="3:18" ht="24" customHeight="1">
       <c r="C23" s="12"/>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="33"/>
-      <c r="O23" s="33"/>
-      <c r="P23" s="33"/>
-      <c r="Q23" s="33"/>
-    </row>
-    <row r="24" spans="3:17">
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-      <c r="N24" s="33"/>
-      <c r="O24" s="33"/>
-      <c r="P24" s="33"/>
-      <c r="Q24" s="33"/>
-    </row>
-    <row r="30" spans="3:17" ht="18.75">
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="34"/>
+      <c r="N23" s="34"/>
+      <c r="O23" s="34"/>
+      <c r="P23" s="34"/>
+      <c r="Q23" s="34"/>
+      <c r="R23" s="34"/>
+    </row>
+    <row r="24" spans="3:18">
+      <c r="K24" s="34"/>
+      <c r="L24" s="34"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="34"/>
+      <c r="O24" s="34"/>
+      <c r="P24" s="34"/>
+      <c r="Q24" s="34"/>
+      <c r="R24" s="34"/>
+    </row>
+    <row r="30" spans="3:18" ht="18.75">
       <c r="C30" s="18" t="s">
         <v>46</v>
       </c>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
     </row>
-    <row r="31" spans="3:17" ht="18.75">
+    <row r="31" spans="3:18" ht="18.75">
       <c r="C31" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D31" s="13"/>
       <c r="E31" s="13"/>
     </row>
-    <row r="32" spans="3:17">
+    <row r="32" spans="3:18">
       <c r="C32" s="12"/>
       <c r="D32" s="13"/>
       <c r="E32" s="13"/>
@@ -3234,7 +3327,7 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="J20:Q24"/>
+    <mergeCell ref="K20:R24"/>
     <mergeCell ref="D9:G9"/>
     <mergeCell ref="D5:G5"/>
     <mergeCell ref="D14:G14"/>
@@ -3252,8 +3345,8 @@
   </sheetPr>
   <dimension ref="B1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3265,17 +3358,17 @@
   <sheetData>
     <row r="1" spans="2:11">
       <c r="B1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="2:11" ht="15.75" thickBot="1"/>
     <row r="3" spans="2:11" ht="26.25" thickBot="1">
       <c r="B3" s="2"/>
       <c r="C3" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>9</v>
@@ -3307,7 +3400,7 @@
         <v>43206</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>31</v>
@@ -3334,7 +3427,7 @@
         <v>43206</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>66</v>
@@ -3352,7 +3445,7 @@
     </row>
     <row r="8" spans="2:11" ht="20.25">
       <c r="B8" s="28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="15.75" thickBot="1"/>
@@ -3362,7 +3455,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>2</v>
@@ -3377,18 +3470,18 @@
         <v>12</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K10" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="2:11">
-      <c r="J11" s="35" t="s">
-        <v>102</v>
+      <c r="J11" s="32" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -3419,19 +3512,19 @@
   <sheetData>
     <row r="1" spans="2:9" ht="24.75" customHeight="1">
       <c r="B1" s="17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="24" customHeight="1">
       <c r="C3" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>38</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G3" s="25">
         <v>43206</v>
@@ -3446,10 +3539,10 @@
       <c r="C5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
     </row>
     <row r="6" spans="2:9" ht="8.25" customHeight="1">
       <c r="C6" s="12"/>
@@ -3465,7 +3558,7 @@
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G7" s="14"/>
     </row>
@@ -3478,10 +3571,10 @@
       <c r="C9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
     </row>
     <row r="10" spans="2:9" ht="9.75" customHeight="1">
       <c r="D10" s="16"/>
@@ -3513,10 +3606,10 @@
       <c r="C14" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
     </row>
     <row r="15" spans="2:9" ht="8.25" customHeight="1">
       <c r="C15" s="12"/>
@@ -3547,59 +3640,59 @@
     </row>
     <row r="19" spans="3:17" ht="24" customHeight="1"/>
     <row r="20" spans="3:17" ht="24" customHeight="1">
-      <c r="J20" s="33" t="s">
+      <c r="J20" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="33"/>
-      <c r="P20" s="33"/>
-      <c r="Q20" s="33"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="34"/>
+      <c r="P20" s="34"/>
+      <c r="Q20" s="34"/>
     </row>
     <row r="21" spans="3:17" ht="24" customHeight="1">
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33"/>
-      <c r="O21" s="33"/>
-      <c r="P21" s="33"/>
-      <c r="Q21" s="33"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="34"/>
+      <c r="P21" s="34"/>
+      <c r="Q21" s="34"/>
     </row>
     <row r="22" spans="3:17" ht="24" customHeight="1">
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="33"/>
-      <c r="Q22" s="33"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="34"/>
+      <c r="P22" s="34"/>
+      <c r="Q22" s="34"/>
     </row>
     <row r="23" spans="3:17" ht="24" customHeight="1">
       <c r="C23" s="12"/>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="33"/>
-      <c r="O23" s="33"/>
-      <c r="P23" s="33"/>
-      <c r="Q23" s="33"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="34"/>
+      <c r="N23" s="34"/>
+      <c r="O23" s="34"/>
+      <c r="P23" s="34"/>
+      <c r="Q23" s="34"/>
     </row>
     <row r="24" spans="3:17">
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-      <c r="N24" s="33"/>
-      <c r="O24" s="33"/>
-      <c r="P24" s="33"/>
-      <c r="Q24" s="33"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="34"/>
+      <c r="L24" s="34"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="34"/>
+      <c r="O24" s="34"/>
+      <c r="P24" s="34"/>
+      <c r="Q24" s="34"/>
     </row>
     <row r="30" spans="3:17" ht="18.75">
       <c r="C30" s="18" t="s">

</xml_diff>

<commit_message>
add product category for Vendor
</commit_message>
<xml_diff>
--- a/doc/界面示意图.xlsx
+++ b/doc/界面示意图.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Storage" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="117">
   <si>
     <t>SN</t>
   </si>
@@ -286,9 +286,6 @@
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>sn</t>
   </si>
   <si>
     <t>Tribul</t>
@@ -404,6 +401,15 @@
   </si>
   <si>
     <t>EEI98</t>
+  </si>
+  <si>
+    <t>Quantity(g)</t>
+  </si>
+  <si>
+    <t>Quantity(Kg)</t>
+  </si>
+  <si>
+    <t>Contacts</t>
   </si>
 </sst>
 </file>
@@ -489,7 +495,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -520,8 +526,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -626,11 +638,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -702,6 +736,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -711,10 +752,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1620,7 +1664,7 @@
   <dimension ref="B1:S39"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28:K29"/>
+      <selection activeCell="M28" sqref="M28:P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1872,6 +1916,9 @@
       <c r="P13" s="10" t="s">
         <v>13</v>
       </c>
+      <c r="Q13" s="37" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="14" spans="2:18" ht="25.5" customHeight="1">
       <c r="B14" s="5" t="s">
@@ -2089,10 +2136,10 @@
         <v>6</v>
       </c>
       <c r="O28" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="P28" s="8" t="s">
         <v>93</v>
-      </c>
-      <c r="P28" s="8" t="s">
-        <v>94</v>
       </c>
       <c r="Q28" s="9" t="s">
         <v>7</v>
@@ -2184,10 +2231,10 @@
     </row>
     <row r="32" spans="2:19">
       <c r="B32" t="s">
+        <v>90</v>
+      </c>
+      <c r="M32" t="s">
         <v>91</v>
-      </c>
-      <c r="M32" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="33" spans="2:12" ht="15.75" thickBot="1"/>
@@ -2207,7 +2254,7 @@
         <v>43</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I34" s="8" t="s">
         <v>12</v>
@@ -2335,61 +2382,61 @@
         <v>43</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="J5" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="36"/>
-      <c r="P5" s="36"/>
-      <c r="Q5" s="36"/>
+      <c r="J5" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+      <c r="N5" s="39"/>
+      <c r="O5" s="39"/>
+      <c r="P5" s="39"/>
+      <c r="Q5" s="39"/>
     </row>
     <row r="6" spans="2:17" ht="8.25" customHeight="1">
       <c r="C6" s="12"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="36"/>
-      <c r="P6" s="36"/>
-      <c r="Q6" s="36"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
+      <c r="P6" s="39"/>
+      <c r="Q6" s="39"/>
     </row>
     <row r="7" spans="2:17" ht="24" customHeight="1">
       <c r="C7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="35" t="s">
-        <v>85</v>
-      </c>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36"/>
-      <c r="N7" s="36"/>
-      <c r="O7" s="36"/>
-      <c r="P7" s="36"/>
-      <c r="Q7" s="36"/>
+      <c r="D7" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="39"/>
+      <c r="O7" s="39"/>
+      <c r="P7" s="39"/>
+      <c r="Q7" s="39"/>
     </row>
     <row r="8" spans="2:17" ht="8.25" customHeight="1">
       <c r="C8" s="12"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="36"/>
-      <c r="O8" s="36"/>
-      <c r="P8" s="36"/>
-      <c r="Q8" s="36"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39"/>
+      <c r="P8" s="39"/>
+      <c r="Q8" s="39"/>
     </row>
     <row r="9" spans="2:17" ht="24" customHeight="1">
       <c r="C9" s="11" t="s">
@@ -2403,14 +2450,14 @@
       <c r="G9" s="14">
         <v>230</v>
       </c>
-      <c r="J9" s="36"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="36"/>
-      <c r="Q9" s="36"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="39"/>
+      <c r="O9" s="39"/>
+      <c r="P9" s="39"/>
+      <c r="Q9" s="39"/>
     </row>
     <row r="10" spans="2:17" ht="8.25" customHeight="1">
       <c r="C10" s="12"/>
@@ -2453,12 +2500,12 @@
       <c r="C15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
       <c r="I15" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="2:17" ht="8.25" customHeight="1">
@@ -2486,10 +2533,10 @@
       <c r="C19" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
     </row>
     <row r="20" spans="3:7" ht="24" customHeight="1">
       <c r="C20" s="12"/>
@@ -2619,7 +2666,7 @@
     </row>
     <row r="10" spans="2:7" ht="24" customHeight="1">
       <c r="C10" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="13"/>
@@ -2649,10 +2696,10 @@
       <c r="C14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
     </row>
     <row r="15" spans="2:7" ht="8.25" customHeight="1">
       <c r="C15" s="12"/>
@@ -2679,10 +2726,10 @@
       <c r="C18" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
     </row>
     <row r="19" spans="2:7" ht="24" customHeight="1">
       <c r="C19" s="12"/>
@@ -2730,7 +2777,7 @@
     </row>
     <row r="29" spans="2:7">
       <c r="C29" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="2:7">
@@ -2866,10 +2913,10 @@
       <c r="C12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
     </row>
     <row r="13" spans="2:7" ht="8.25" customHeight="1">
       <c r="C13" s="12"/>
@@ -2896,10 +2943,10 @@
       <c r="C16" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
     </row>
     <row r="17" spans="2:5" ht="24" customHeight="1">
       <c r="C17" s="12"/>
@@ -2930,7 +2977,7 @@
     <row r="21" spans="2:5" ht="24" customHeight="1">
       <c r="B21" s="18"/>
       <c r="C21" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
@@ -2959,36 +3006,38 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="B1:K12"/>
+  <dimension ref="B1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:H4"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="22" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" customWidth="1"/>
+    <col min="4" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11">
+    <row r="1" spans="2:13">
       <c r="B1" t="s">
         <v>58</v>
       </c>
       <c r="D1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" t="s">
         <v>111</v>
       </c>
-      <c r="F1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="2:11" ht="15.75" thickBot="1"/>
-    <row r="3" spans="2:11" ht="15.75" thickBot="1">
+    </row>
+    <row r="2" spans="2:13" ht="15.75" thickBot="1"/>
+    <row r="3" spans="2:13" ht="15.75" thickBot="1">
       <c r="B3" s="2"/>
       <c r="C3" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>59</v>
@@ -2996,26 +3045,32 @@
       <c r="E3" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="G3" s="8" t="s">
+      <c r="F3" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="K3" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="J3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="10" t="s">
+      <c r="L3" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="M3" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="25.5" customHeight="1">
+    <row r="4" spans="2:13" ht="25.5" customHeight="1">
       <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
@@ -3028,26 +3083,30 @@
       <c r="E4" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="43"/>
+      <c r="G4" s="4">
+        <v>3</v>
+      </c>
+      <c r="H4" s="29">
         <v>1</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="J4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="6">
+      <c r="K4" s="6">
         <v>13</v>
       </c>
-      <c r="J4" s="6">
+      <c r="L4" s="6">
         <v>100</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="M4" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="25.5" customHeight="1">
+    <row r="5" spans="2:13" ht="25.5" customHeight="1">
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
@@ -3060,57 +3119,70 @@
       <c r="E5" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="43"/>
+      <c r="G5" s="4">
+        <v>3</v>
+      </c>
+      <c r="H5" s="29">
         <v>2</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="J5" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="I5" s="6">
+      <c r="K5" s="6">
         <v>45</v>
       </c>
-      <c r="J5" s="6">
+      <c r="L5" s="6">
         <v>30</v>
       </c>
-      <c r="K5" s="6"/>
-    </row>
-    <row r="8" spans="2:11">
+      <c r="M5" s="6"/>
+    </row>
+    <row r="8" spans="2:13">
       <c r="B8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="15.75" thickBot="1"/>
-    <row r="10" spans="2:11" ht="26.25" thickBot="1">
+    <row r="9" spans="2:13" ht="15.75" thickBot="1"/>
+    <row r="10" spans="2:13" ht="26.25" thickBot="1">
       <c r="B10" s="2"/>
       <c r="C10" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>104</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>105</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="J10" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="K10" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="10" t="s">
+      <c r="L10" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="M10" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:11">
+    <row r="11" spans="2:13">
       <c r="B11" s="5" t="s">
         <v>14</v>
       </c>
@@ -3123,21 +3195,28 @@
       <c r="E11" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="43"/>
+      <c r="G11" s="6">
+        <v>3</v>
+      </c>
+      <c r="H11" s="29">
+        <v>1</v>
+      </c>
+      <c r="I11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="J11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="6">
-        <v>13</v>
-      </c>
-      <c r="I11" s="6">
-        <v>100</v>
-      </c>
-      <c r="J11" s="6"/>
-    </row>
-    <row r="12" spans="2:11">
+      <c r="K11" s="6">
+        <v>0</v>
+      </c>
+      <c r="L11" s="6">
+        <v>10</v>
+      </c>
+      <c r="M11" s="6"/>
+    </row>
+    <row r="12" spans="2:13">
       <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
@@ -3150,19 +3229,26 @@
       <c r="E12" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="43"/>
+      <c r="G12" s="6">
+        <v>3</v>
+      </c>
+      <c r="H12" s="29">
+        <v>2</v>
+      </c>
+      <c r="I12" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="J12" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="H12" s="6">
-        <v>45</v>
-      </c>
-      <c r="I12" s="6">
-        <v>30</v>
-      </c>
-      <c r="J12" s="6"/>
+      <c r="K12" s="6">
+        <v>0</v>
+      </c>
+      <c r="L12" s="6">
+        <v>10</v>
+      </c>
+      <c r="M12" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3177,7 +3263,7 @@
   </sheetPr>
   <dimension ref="B1:U44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C22" workbookViewId="0">
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
@@ -3202,7 +3288,7 @@
     </row>
     <row r="2" spans="2:10">
       <c r="F2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="24" customHeight="1">
@@ -3229,10 +3315,10 @@
       <c r="C5" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
     </row>
     <row r="6" spans="2:10" ht="8.25" customHeight="1">
       <c r="C6" s="12"/>
@@ -3261,10 +3347,10 @@
       <c r="C9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
       <c r="J9" t="s">
         <v>70</v>
       </c>
@@ -3285,7 +3371,7 @@
         <v>2</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="11"/>
@@ -3294,7 +3380,7 @@
         <v>82</v>
       </c>
       <c r="J12" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="8.25" customHeight="1">
@@ -3306,17 +3392,17 @@
       <c r="C14" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
+      <c r="D14" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
       <c r="I14" s="34" t="s">
         <v>83</v>
       </c>
       <c r="J14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="8.25" customHeight="1">
@@ -3373,7 +3459,7 @@
         <v>33</v>
       </c>
       <c r="K19" s="31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L19" s="31" t="s">
         <v>36</v>
@@ -3386,59 +3472,59 @@
       </c>
     </row>
     <row r="20" spans="3:21" ht="24" customHeight="1">
-      <c r="K20" s="36" t="s">
+      <c r="K20" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="L20" s="36"/>
-      <c r="M20" s="36"/>
-      <c r="N20" s="36"/>
-      <c r="O20" s="36"/>
-      <c r="P20" s="36"/>
-      <c r="Q20" s="36"/>
-      <c r="R20" s="36"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="39"/>
+      <c r="O20" s="39"/>
+      <c r="P20" s="39"/>
+      <c r="Q20" s="39"/>
+      <c r="R20" s="39"/>
     </row>
     <row r="21" spans="3:21" ht="24" customHeight="1">
-      <c r="K21" s="36"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="36"/>
-      <c r="O21" s="36"/>
-      <c r="P21" s="36"/>
-      <c r="Q21" s="36"/>
-      <c r="R21" s="36"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="39"/>
+      <c r="P21" s="39"/>
+      <c r="Q21" s="39"/>
+      <c r="R21" s="39"/>
     </row>
     <row r="22" spans="3:21" ht="24" customHeight="1">
-      <c r="K22" s="36"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="36"/>
-      <c r="N22" s="36"/>
-      <c r="O22" s="36"/>
-      <c r="P22" s="36"/>
-      <c r="Q22" s="36"/>
-      <c r="R22" s="36"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="39"/>
+      <c r="O22" s="39"/>
+      <c r="P22" s="39"/>
+      <c r="Q22" s="39"/>
+      <c r="R22" s="39"/>
     </row>
     <row r="23" spans="3:21" ht="24" customHeight="1">
       <c r="C23" s="12"/>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
-      <c r="K23" s="36"/>
-      <c r="L23" s="36"/>
-      <c r="M23" s="36"/>
-      <c r="N23" s="36"/>
-      <c r="O23" s="36"/>
-      <c r="P23" s="36"/>
-      <c r="Q23" s="36"/>
-      <c r="R23" s="36"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="39"/>
+      <c r="O23" s="39"/>
+      <c r="P23" s="39"/>
+      <c r="Q23" s="39"/>
+      <c r="R23" s="39"/>
     </row>
     <row r="24" spans="3:21">
-      <c r="K24" s="36"/>
-      <c r="L24" s="36"/>
-      <c r="M24" s="36"/>
-      <c r="N24" s="36"/>
-      <c r="O24" s="36"/>
-      <c r="P24" s="36"/>
-      <c r="Q24" s="36"/>
-      <c r="R24" s="36"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="39"/>
+      <c r="O24" s="39"/>
+      <c r="P24" s="39"/>
+      <c r="Q24" s="39"/>
+      <c r="R24" s="39"/>
     </row>
     <row r="28" spans="3:21">
       <c r="Q28" s="11" t="s">
@@ -3519,7 +3605,7 @@
     </row>
     <row r="36" spans="3:21" ht="26.25">
       <c r="P36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q36" s="11" t="s">
         <v>2</v>
@@ -3594,7 +3680,7 @@
   <dimension ref="B1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="J3" sqref="J3:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3625,7 +3711,7 @@
       <c r="F3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="35" t="s">
         <v>3</v>
       </c>
       <c r="H3" s="8" t="s">
@@ -3635,7 +3721,7 @@
         <v>12</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>13</v>
@@ -3657,7 +3743,7 @@
       <c r="F4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="G4" s="36" t="s">
         <v>32</v>
       </c>
       <c r="H4" s="6">
@@ -3687,7 +3773,7 @@
       <c r="F5" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G5" s="39" t="s">
+      <c r="G5" s="36" t="s">
         <v>67</v>
       </c>
       <c r="H5" s="6">
@@ -3713,7 +3799,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>9</v>
@@ -3734,10 +3820,10 @@
         <v>12</v>
       </c>
       <c r="K10" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="L10" s="10" t="s">
         <v>97</v>
-      </c>
-      <c r="L10" s="10" t="s">
-        <v>98</v>
       </c>
       <c r="M10" s="10" t="s">
         <v>13</v>
@@ -3745,7 +3831,7 @@
     </row>
     <row r="11" spans="2:13">
       <c r="K11" s="32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -3803,10 +3889,10 @@
       <c r="C5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
     </row>
     <row r="6" spans="2:9" ht="8.25" customHeight="1">
       <c r="C6" s="12"/>
@@ -3835,10 +3921,10 @@
       <c r="C9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
     </row>
     <row r="10" spans="2:9" ht="9.75" customHeight="1">
       <c r="D10" s="16"/>
@@ -3870,10 +3956,10 @@
       <c r="C14" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
     </row>
     <row r="15" spans="2:9" ht="8.25" customHeight="1">
       <c r="C15" s="12"/>
@@ -3904,59 +3990,59 @@
     </row>
     <row r="19" spans="3:17" ht="24" customHeight="1"/>
     <row r="20" spans="3:17" ht="24" customHeight="1">
-      <c r="J20" s="36" t="s">
+      <c r="J20" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="36"/>
-      <c r="N20" s="36"/>
-      <c r="O20" s="36"/>
-      <c r="P20" s="36"/>
-      <c r="Q20" s="36"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="39"/>
+      <c r="O20" s="39"/>
+      <c r="P20" s="39"/>
+      <c r="Q20" s="39"/>
     </row>
     <row r="21" spans="3:17" ht="24" customHeight="1">
-      <c r="J21" s="36"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="36"/>
-      <c r="O21" s="36"/>
-      <c r="P21" s="36"/>
-      <c r="Q21" s="36"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="39"/>
+      <c r="P21" s="39"/>
+      <c r="Q21" s="39"/>
     </row>
     <row r="22" spans="3:17" ht="24" customHeight="1">
-      <c r="J22" s="36"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="36"/>
-      <c r="N22" s="36"/>
-      <c r="O22" s="36"/>
-      <c r="P22" s="36"/>
-      <c r="Q22" s="36"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="39"/>
+      <c r="O22" s="39"/>
+      <c r="P22" s="39"/>
+      <c r="Q22" s="39"/>
     </row>
     <row r="23" spans="3:17" ht="24" customHeight="1">
       <c r="C23" s="12"/>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
-      <c r="J23" s="36"/>
-      <c r="K23" s="36"/>
-      <c r="L23" s="36"/>
-      <c r="M23" s="36"/>
-      <c r="N23" s="36"/>
-      <c r="O23" s="36"/>
-      <c r="P23" s="36"/>
-      <c r="Q23" s="36"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="39"/>
+      <c r="O23" s="39"/>
+      <c r="P23" s="39"/>
+      <c r="Q23" s="39"/>
     </row>
     <row r="24" spans="3:17">
-      <c r="J24" s="36"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="36"/>
-      <c r="M24" s="36"/>
-      <c r="N24" s="36"/>
-      <c r="O24" s="36"/>
-      <c r="P24" s="36"/>
-      <c r="Q24" s="36"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="39"/>
+      <c r="N24" s="39"/>
+      <c r="O24" s="39"/>
+      <c r="P24" s="39"/>
+      <c r="Q24" s="39"/>
     </row>
     <row r="30" spans="3:17" ht="18.75">
       <c r="C30" s="18" t="s">
@@ -4002,7 +4088,7 @@
   </sheetPr>
   <dimension ref="B1:Q30"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -4022,14 +4108,14 @@
     </row>
     <row r="3" spans="2:10" ht="24" customHeight="1">
       <c r="C3" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>38</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G3" s="25">
         <v>43206</v>
@@ -4044,10 +4130,10 @@
       <c r="C5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
     </row>
     <row r="6" spans="2:10" ht="9.75" customHeight="1">
       <c r="D6" s="16"/>
@@ -4076,10 +4162,10 @@
       <c r="C9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
     </row>
     <row r="10" spans="2:10" ht="8.25" customHeight="1">
       <c r="C10" s="12"/>
@@ -4105,7 +4191,7 @@
     </row>
     <row r="13" spans="2:10" ht="24" customHeight="1">
       <c r="C13" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D13" s="14">
         <v>3</v>
@@ -4125,72 +4211,72 @@
       <c r="C15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
     </row>
     <row r="16" spans="2:10" ht="24" customHeight="1"/>
     <row r="17" spans="3:17" ht="24" customHeight="1">
-      <c r="J17" s="36" t="s">
+      <c r="J17" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="K17" s="36"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="36"/>
-      <c r="N17" s="36"/>
-      <c r="O17" s="36"/>
-      <c r="P17" s="36"/>
-      <c r="Q17" s="36"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="39"/>
+      <c r="N17" s="39"/>
+      <c r="O17" s="39"/>
+      <c r="P17" s="39"/>
+      <c r="Q17" s="39"/>
     </row>
     <row r="18" spans="3:17" ht="24" customHeight="1">
       <c r="C18" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="J18" s="36"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="36"/>
-      <c r="N18" s="36"/>
-      <c r="O18" s="36"/>
-      <c r="P18" s="36"/>
-      <c r="Q18" s="36"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="39"/>
+      <c r="N18" s="39"/>
+      <c r="O18" s="39"/>
+      <c r="P18" s="39"/>
+      <c r="Q18" s="39"/>
     </row>
     <row r="19" spans="3:17" ht="24" customHeight="1">
       <c r="C19" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="J19" s="36"/>
-      <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="36"/>
-      <c r="N19" s="36"/>
-      <c r="O19" s="36"/>
-      <c r="P19" s="36"/>
-      <c r="Q19" s="36"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="39"/>
+      <c r="P19" s="39"/>
+      <c r="Q19" s="39"/>
     </row>
     <row r="20" spans="3:17" ht="24" customHeight="1">
       <c r="C20" s="12"/>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="36"/>
-      <c r="N20" s="36"/>
-      <c r="O20" s="36"/>
-      <c r="P20" s="36"/>
-      <c r="Q20" s="36"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="39"/>
+      <c r="O20" s="39"/>
+      <c r="P20" s="39"/>
+      <c r="Q20" s="39"/>
     </row>
     <row r="21" spans="3:17">
-      <c r="J21" s="36"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="36"/>
-      <c r="O21" s="36"/>
-      <c r="P21" s="36"/>
-      <c r="Q21" s="36"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="39"/>
+      <c r="P21" s="39"/>
+      <c r="Q21" s="39"/>
     </row>
     <row r="27" spans="3:17">
       <c r="D27" s="13"/>

</xml_diff>

<commit_message>
modify stock and add query productInventory
</commit_message>
<xml_diff>
--- a/doc/界面示意图.xlsx
+++ b/doc/界面示意图.xlsx
@@ -771,6 +771,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -779,13 +786,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1692,7 +1692,7 @@
   <dimension ref="B1:S39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1947,7 +1947,7 @@
       <c r="Q13" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="R13" s="48" t="s">
+      <c r="R13" s="45" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1959,10 +1959,10 @@
       <c r="D14" s="6">
         <v>1</v>
       </c>
-      <c r="E14" s="44">
+      <c r="E14" s="41">
         <v>43206</v>
       </c>
-      <c r="F14" s="45" t="s">
+      <c r="F14" s="42" t="s">
         <v>31</v>
       </c>
       <c r="G14" s="6" t="s">
@@ -1971,30 +1971,30 @@
       <c r="H14" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="I14" s="45" t="s">
+      <c r="I14" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="J14" s="47" t="s">
+      <c r="J14" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="K14" s="47">
+      <c r="K14" s="44">
         <v>0.01</v>
       </c>
-      <c r="L14" s="47" t="s">
+      <c r="L14" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="M14" s="47" t="s">
+      <c r="M14" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="N14" s="47">
+      <c r="N14" s="44">
         <v>203</v>
       </c>
-      <c r="O14" s="45">
+      <c r="O14" s="42">
         <v>50</v>
       </c>
-      <c r="P14" s="45"/>
-      <c r="Q14" s="46"/>
-      <c r="R14" s="46"/>
+      <c r="P14" s="42"/>
+      <c r="Q14" s="43"/>
+      <c r="R14" s="43"/>
     </row>
     <row r="15" spans="2:18" ht="25.5" customHeight="1">
       <c r="B15" s="3" t="s">
@@ -2415,61 +2415,61 @@
         <v>43</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="J5" s="42" t="s">
+      <c r="J5" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="42"/>
-      <c r="O5" s="42"/>
-      <c r="P5" s="42"/>
-      <c r="Q5" s="42"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="47"/>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="47"/>
     </row>
     <row r="6" spans="2:17" ht="8.25" customHeight="1">
       <c r="C6" s="12"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="42"/>
-      <c r="O6" s="42"/>
-      <c r="P6" s="42"/>
-      <c r="Q6" s="42"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="47"/>
+      <c r="P6" s="47"/>
+      <c r="Q6" s="47"/>
     </row>
     <row r="7" spans="2:17" ht="24" customHeight="1">
       <c r="C7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
-      <c r="M7" s="42"/>
-      <c r="N7" s="42"/>
-      <c r="O7" s="42"/>
-      <c r="P7" s="42"/>
-      <c r="Q7" s="42"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="47"/>
+      <c r="P7" s="47"/>
+      <c r="Q7" s="47"/>
     </row>
     <row r="8" spans="2:17" ht="8.25" customHeight="1">
       <c r="C8" s="12"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="42"/>
-      <c r="O8" s="42"/>
-      <c r="P8" s="42"/>
-      <c r="Q8" s="42"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="47"/>
+      <c r="P8" s="47"/>
+      <c r="Q8" s="47"/>
     </row>
     <row r="9" spans="2:17" ht="24" customHeight="1">
       <c r="C9" s="11" t="s">
@@ -2483,14 +2483,14 @@
       <c r="G9" s="14">
         <v>230</v>
       </c>
-      <c r="J9" s="42"/>
-      <c r="K9" s="42"/>
-      <c r="L9" s="42"/>
-      <c r="M9" s="42"/>
-      <c r="N9" s="42"/>
-      <c r="O9" s="42"/>
-      <c r="P9" s="42"/>
-      <c r="Q9" s="42"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="47"/>
+      <c r="P9" s="47"/>
+      <c r="Q9" s="47"/>
     </row>
     <row r="10" spans="2:17" ht="8.25" customHeight="1">
       <c r="C10" s="12"/>
@@ -2533,10 +2533,10 @@
       <c r="C15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
       <c r="I15" s="30" t="s">
         <v>86</v>
       </c>
@@ -2566,10 +2566,10 @@
       <c r="C19" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
     </row>
     <row r="20" spans="3:7" ht="24" customHeight="1">
       <c r="C20" s="12"/>
@@ -2729,10 +2729,10 @@
       <c r="C14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
     </row>
     <row r="15" spans="2:7" ht="8.25" customHeight="1">
       <c r="C15" s="12"/>
@@ -2759,10 +2759,10 @@
       <c r="C18" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
     </row>
     <row r="19" spans="2:7" ht="24" customHeight="1">
       <c r="C19" s="12"/>
@@ -2946,10 +2946,10 @@
       <c r="C12" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
     </row>
     <row r="13" spans="2:7" ht="8.25" customHeight="1">
       <c r="C13" s="12"/>
@@ -2976,10 +2976,10 @@
       <c r="C16" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
     </row>
     <row r="17" spans="2:5" ht="24" customHeight="1">
       <c r="C17" s="12"/>
@@ -3348,10 +3348,10 @@
       <c r="C5" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
     </row>
     <row r="6" spans="2:10" ht="8.25" customHeight="1">
       <c r="C6" s="12"/>
@@ -3380,10 +3380,10 @@
       <c r="C9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
       <c r="J9" t="s">
         <v>70</v>
       </c>
@@ -3425,12 +3425,12 @@
       <c r="C14" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
       <c r="I14" s="34" t="s">
         <v>83</v>
       </c>
@@ -3505,59 +3505,59 @@
       </c>
     </row>
     <row r="20" spans="3:21" ht="24" customHeight="1">
-      <c r="K20" s="42" t="s">
+      <c r="K20" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="L20" s="42"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="42"/>
-      <c r="O20" s="42"/>
-      <c r="P20" s="42"/>
-      <c r="Q20" s="42"/>
-      <c r="R20" s="42"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="47"/>
+      <c r="O20" s="47"/>
+      <c r="P20" s="47"/>
+      <c r="Q20" s="47"/>
+      <c r="R20" s="47"/>
     </row>
     <row r="21" spans="3:21" ht="24" customHeight="1">
-      <c r="K21" s="42"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="42"/>
-      <c r="P21" s="42"/>
-      <c r="Q21" s="42"/>
-      <c r="R21" s="42"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="47"/>
+      <c r="P21" s="47"/>
+      <c r="Q21" s="47"/>
+      <c r="R21" s="47"/>
     </row>
     <row r="22" spans="3:21" ht="24" customHeight="1">
-      <c r="K22" s="42"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="42"/>
-      <c r="O22" s="42"/>
-      <c r="P22" s="42"/>
-      <c r="Q22" s="42"/>
-      <c r="R22" s="42"/>
+      <c r="K22" s="47"/>
+      <c r="L22" s="47"/>
+      <c r="M22" s="47"/>
+      <c r="N22" s="47"/>
+      <c r="O22" s="47"/>
+      <c r="P22" s="47"/>
+      <c r="Q22" s="47"/>
+      <c r="R22" s="47"/>
     </row>
     <row r="23" spans="3:21" ht="24" customHeight="1">
       <c r="C23" s="12"/>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
-      <c r="K23" s="42"/>
-      <c r="L23" s="42"/>
-      <c r="M23" s="42"/>
-      <c r="N23" s="42"/>
-      <c r="O23" s="42"/>
-      <c r="P23" s="42"/>
-      <c r="Q23" s="42"/>
-      <c r="R23" s="42"/>
+      <c r="K23" s="47"/>
+      <c r="L23" s="47"/>
+      <c r="M23" s="47"/>
+      <c r="N23" s="47"/>
+      <c r="O23" s="47"/>
+      <c r="P23" s="47"/>
+      <c r="Q23" s="47"/>
+      <c r="R23" s="47"/>
     </row>
     <row r="24" spans="3:21">
-      <c r="K24" s="42"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="42"/>
-      <c r="O24" s="42"/>
-      <c r="P24" s="42"/>
-      <c r="Q24" s="42"/>
-      <c r="R24" s="42"/>
+      <c r="K24" s="47"/>
+      <c r="L24" s="47"/>
+      <c r="M24" s="47"/>
+      <c r="N24" s="47"/>
+      <c r="O24" s="47"/>
+      <c r="P24" s="47"/>
+      <c r="Q24" s="47"/>
+      <c r="R24" s="47"/>
     </row>
     <row r="28" spans="3:21">
       <c r="Q28" s="11" t="s">
@@ -3922,10 +3922,10 @@
       <c r="C5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
     </row>
     <row r="6" spans="2:9" ht="8.25" customHeight="1">
       <c r="C6" s="12"/>
@@ -3954,10 +3954,10 @@
       <c r="C9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
     </row>
     <row r="10" spans="2:9" ht="9.75" customHeight="1">
       <c r="D10" s="16"/>
@@ -3989,10 +3989,10 @@
       <c r="C14" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
     </row>
     <row r="15" spans="2:9" ht="8.25" customHeight="1">
       <c r="C15" s="12"/>
@@ -4023,59 +4023,59 @@
     </row>
     <row r="19" spans="3:17" ht="24" customHeight="1"/>
     <row r="20" spans="3:17" ht="24" customHeight="1">
-      <c r="J20" s="42" t="s">
+      <c r="J20" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="K20" s="42"/>
-      <c r="L20" s="42"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="42"/>
-      <c r="O20" s="42"/>
-      <c r="P20" s="42"/>
-      <c r="Q20" s="42"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="47"/>
+      <c r="O20" s="47"/>
+      <c r="P20" s="47"/>
+      <c r="Q20" s="47"/>
     </row>
     <row r="21" spans="3:17" ht="24" customHeight="1">
-      <c r="J21" s="42"/>
-      <c r="K21" s="42"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="42"/>
-      <c r="P21" s="42"/>
-      <c r="Q21" s="42"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="47"/>
+      <c r="P21" s="47"/>
+      <c r="Q21" s="47"/>
     </row>
     <row r="22" spans="3:17" ht="24" customHeight="1">
-      <c r="J22" s="42"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="42"/>
-      <c r="O22" s="42"/>
-      <c r="P22" s="42"/>
-      <c r="Q22" s="42"/>
+      <c r="J22" s="47"/>
+      <c r="K22" s="47"/>
+      <c r="L22" s="47"/>
+      <c r="M22" s="47"/>
+      <c r="N22" s="47"/>
+      <c r="O22" s="47"/>
+      <c r="P22" s="47"/>
+      <c r="Q22" s="47"/>
     </row>
     <row r="23" spans="3:17" ht="24" customHeight="1">
       <c r="C23" s="12"/>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="42"/>
-      <c r="L23" s="42"/>
-      <c r="M23" s="42"/>
-      <c r="N23" s="42"/>
-      <c r="O23" s="42"/>
-      <c r="P23" s="42"/>
-      <c r="Q23" s="42"/>
+      <c r="J23" s="47"/>
+      <c r="K23" s="47"/>
+      <c r="L23" s="47"/>
+      <c r="M23" s="47"/>
+      <c r="N23" s="47"/>
+      <c r="O23" s="47"/>
+      <c r="P23" s="47"/>
+      <c r="Q23" s="47"/>
     </row>
     <row r="24" spans="3:17">
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="42"/>
-      <c r="O24" s="42"/>
-      <c r="P24" s="42"/>
-      <c r="Q24" s="42"/>
+      <c r="J24" s="47"/>
+      <c r="K24" s="47"/>
+      <c r="L24" s="47"/>
+      <c r="M24" s="47"/>
+      <c r="N24" s="47"/>
+      <c r="O24" s="47"/>
+      <c r="P24" s="47"/>
+      <c r="Q24" s="47"/>
     </row>
     <row r="30" spans="3:17" ht="18.75">
       <c r="C30" s="18" t="s">
@@ -4163,10 +4163,10 @@
       <c r="C5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
     </row>
     <row r="6" spans="2:10" ht="9.75" customHeight="1">
       <c r="D6" s="16"/>
@@ -4195,10 +4195,10 @@
       <c r="C9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
     </row>
     <row r="10" spans="2:10" ht="8.25" customHeight="1">
       <c r="C10" s="12"/>
@@ -4244,72 +4244,72 @@
       <c r="C15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
     </row>
     <row r="16" spans="2:10" ht="24" customHeight="1"/>
     <row r="17" spans="3:17" ht="24" customHeight="1">
-      <c r="J17" s="42" t="s">
+      <c r="J17" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="K17" s="42"/>
-      <c r="L17" s="42"/>
-      <c r="M17" s="42"/>
-      <c r="N17" s="42"/>
-      <c r="O17" s="42"/>
-      <c r="P17" s="42"/>
-      <c r="Q17" s="42"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="47"/>
+      <c r="O17" s="47"/>
+      <c r="P17" s="47"/>
+      <c r="Q17" s="47"/>
     </row>
     <row r="18" spans="3:17" ht="24" customHeight="1">
       <c r="C18" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="J18" s="42"/>
-      <c r="K18" s="42"/>
-      <c r="L18" s="42"/>
-      <c r="M18" s="42"/>
-      <c r="N18" s="42"/>
-      <c r="O18" s="42"/>
-      <c r="P18" s="42"/>
-      <c r="Q18" s="42"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="47"/>
+      <c r="M18" s="47"/>
+      <c r="N18" s="47"/>
+      <c r="O18" s="47"/>
+      <c r="P18" s="47"/>
+      <c r="Q18" s="47"/>
     </row>
     <row r="19" spans="3:17" ht="24" customHeight="1">
       <c r="C19" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="J19" s="42"/>
-      <c r="K19" s="42"/>
-      <c r="L19" s="42"/>
-      <c r="M19" s="42"/>
-      <c r="N19" s="42"/>
-      <c r="O19" s="42"/>
-      <c r="P19" s="42"/>
-      <c r="Q19" s="42"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="47"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="47"/>
+      <c r="N19" s="47"/>
+      <c r="O19" s="47"/>
+      <c r="P19" s="47"/>
+      <c r="Q19" s="47"/>
     </row>
     <row r="20" spans="3:17" ht="24" customHeight="1">
       <c r="C20" s="12"/>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
-      <c r="L20" s="42"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="42"/>
-      <c r="O20" s="42"/>
-      <c r="P20" s="42"/>
-      <c r="Q20" s="42"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="47"/>
+      <c r="O20" s="47"/>
+      <c r="P20" s="47"/>
+      <c r="Q20" s="47"/>
     </row>
     <row r="21" spans="3:17">
-      <c r="J21" s="42"/>
-      <c r="K21" s="42"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="42"/>
-      <c r="P21" s="42"/>
-      <c r="Q21" s="42"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="47"/>
+      <c r="P21" s="47"/>
+      <c r="Q21" s="47"/>
     </row>
     <row r="27" spans="3:17">
       <c r="D27" s="13"/>

</xml_diff>